<commit_message>
Debugging for Export Code
Needed to fix some data type stuff and only use non-NAN variables.
</commit_message>
<xml_diff>
--- a/BalloonData_1obj.xlsx
+++ b/BalloonData_1obj.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuliannaEvans\Documents\MATLAB\balloonGit\testCustomFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuliannaEvans\Documents\MATLAB\balloonGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870BB37A-CDA9-43FC-AB6A-2EBBEA800D52}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{2E0B384F-50F2-4DD8-B093-089C4CD4DEF5}"/>
   </bookViews>
@@ -47,7 +48,7 @@
     <t>balloon1</t>
   </si>
   <si>
-    <t>27 Feb 2018 16:00:00.000'</t>
+    <t>18 Mar 2018 16:00:00.000'</t>
   </si>
 </sst>
 </file>
@@ -403,7 +404,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Data Download Reorg 3
Pretty much everything working now. Throwing errors on the indexing, but that's because I have latitudes/longitudes outside of the AT, which needs Monte Carlo stuff. Used randi() for now
</commit_message>
<xml_diff>
--- a/BalloonData_1obj.xlsx
+++ b/BalloonData_1obj.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuliannaEvans\Documents\MATLAB\balloonGit\testCustomFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuliannaEvans\Documents\MATLAB\balloonGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A25D62-15A5-436D-8E1C-2E0500FB5903}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{2E0B384F-50F2-4DD8-B093-089C4CD4DEF5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5628" xr2:uid="{2E0B384F-50F2-4DD8-B093-089C4CD4DEF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,7 +48,7 @@
     <t>balloon1</t>
   </si>
   <si>
-    <t>27 Feb 2018 16:00:00.000'</t>
+    <t>11 Apr 2018 16:00:00.000'</t>
   </si>
 </sst>
 </file>
@@ -403,10 +404,15 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -436,10 +442,10 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2">
-        <v>-80</v>
+        <v>-104</v>
       </c>
       <c r="E2">
         <v>0</v>

</xml_diff>